<commit_message>
SC3211 / SC3212 작업
</commit_message>
<xml_diff>
--- a/lsNikko.MES(19.10.01~20.07)/개발일정관리/작업리스트.xlsx
+++ b/lsNikko.MES(19.10.01~20.07)/개발일정관리/작업리스트.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\good4\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_FiveM_WorkSpace\lsNikko.MES(19.10.01~20.07)\개발일정관리\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871733FB-C9EE-4600-B973-0154815124A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DF786D-116B-4D9F-AFBF-85700F057C31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="489" xr2:uid="{BA8A56E4-647E-4669-9F98-C06DEFE6D1A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="173">
   <si>
     <t>프로세스</t>
   </si>
@@ -630,6 +630,42 @@
   </si>
   <si>
     <t>SC3215</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC2343</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC3210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC3211</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC3212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-01-01 ~ 2020-02-10 까지 테스트 데이터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타제품재고조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubTotal 쿼리 짜야 할 듯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기간별재고조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동정광재고현황조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1397,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB16A3E-7B95-4A31-91C1-D685BA0F5D49}">
-  <dimension ref="A1:U68"/>
+  <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3628,7 +3664,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B65" s="27" t="s">
         <v>124</v>
       </c>
@@ -3639,7 +3675,7 @@
         <v>43826</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B66" s="27" t="s">
         <v>126</v>
       </c>
@@ -3650,7 +3686,7 @@
         <v>43832</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B67" s="27" t="s">
         <v>127</v>
       </c>
@@ -3661,12 +3697,56 @@
         <v>43832</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B68" s="27" t="s">
         <v>128</v>
       </c>
       <c r="C68" s="29" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B69" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="G69" s="28">
+        <v>43837</v>
+      </c>
+      <c r="H69" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B70" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="G70" s="28">
+        <v>43838</v>
+      </c>
+      <c r="H70" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="B71" s="27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="B72" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72" t="s">
+        <v>169</v>
+      </c>
+      <c r="H72" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>